<commit_message>
Updated the framework code
</commit_message>
<xml_diff>
--- a/UFT Framework/Controller.xlsx
+++ b/UFT Framework/Controller.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87188231-BD08-40C1-992F-2794C7F78E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DDDE5E-BDD5-4463-88EC-E728F44D1E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20160" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="20160" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Browser</t>
   </si>
@@ -80,13 +80,25 @@
   </si>
   <si>
     <t>HTML</t>
+  </si>
+  <si>
+    <t>Test_03</t>
+  </si>
+  <si>
+    <t>Test_04</t>
+  </si>
+  <si>
+    <t>Test_05</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +118,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -531,11 +549,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,7 +629,71 @@
       </c>
       <c r="G3" s="7"/>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added script for admin model
</commit_message>
<xml_diff>
--- a/UFT Framework/Controller.xlsx
+++ b/UFT Framework/Controller.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DDDE5E-BDD5-4463-88EC-E728F44D1E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3CBA3C-27C9-45EE-AF9E-78075ADA010E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="3900" windowWidth="20160" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="20160" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
   <si>
     <t>Browser</t>
   </si>
@@ -70,28 +70,31 @@
     <t>http://3.65.165.176:8082/Xe/</t>
   </si>
   <si>
-    <t>Test_02</t>
-  </si>
-  <si>
-    <t>Test_01</t>
-  </si>
-  <si>
     <t>Report type</t>
   </si>
   <si>
     <t>HTML</t>
   </si>
   <si>
-    <t>Test_03</t>
-  </si>
-  <si>
-    <t>Test_04</t>
-  </si>
-  <si>
-    <t>Test_05</t>
-  </si>
-  <si>
-    <t>FAIL</t>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>02_Administrative_Profiles_View_Edit_Remove_details</t>
+  </si>
+  <si>
+    <t>03_Administrative_System_Rights_Create_Search_Remove</t>
+  </si>
+  <si>
+    <t>04_Administrative_Profile_Permissions_Filters_Enable_Disable_Inherit_Rollback</t>
+  </si>
+  <si>
+    <t>05_Administrative_Password_Policy</t>
+  </si>
+  <si>
+    <t>06_Administrative_Audit_Trail</t>
+  </si>
+  <si>
+    <t>01_Administrative_CreateNewUser</t>
   </si>
 </sst>
 </file>
@@ -195,7 +198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -207,7 +210,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -549,16 +559,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:A6"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="43.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="74.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
@@ -574,16 +585,16 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -594,19 +605,19 @@
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>18</v>
+      <c r="C2" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
@@ -615,19 +626,19 @@
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
+      <c r="C3" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
@@ -636,19 +647,19 @@
       <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
@@ -657,19 +668,19 @@
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
@@ -678,19 +689,40 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -726,7 +758,7 @@
         <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,7 +772,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added scripts for Scheme set up
</commit_message>
<xml_diff>
--- a/UFT Framework/Controller.xlsx
+++ b/UFT Framework/Controller.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3CBA3C-27C9-45EE-AF9E-78075ADA010E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA1F12-4ECB-4BA9-AE94-4A9E57867D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3120" yWindow="3120" windowWidth="20160" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27120" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
   <si>
     <t>Browser</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>DEV1</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -95,13 +89,40 @@
   </si>
   <si>
     <t>01_Administrative_CreateNewUser</t>
+  </si>
+  <si>
+    <t>08_Scheme_Create_New_Sponsor_Approve_addCostCenter_RemoveSponsor</t>
+  </si>
+  <si>
+    <t>09_Scheme_Basic_Setup_ModuleAllowanceConfigurations_DateAnd InsuranceCovers</t>
+  </si>
+  <si>
+    <t>07_Scheme_Setup_CreateNewScheme_Approve_Clone_Switch</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>AppURL</t>
+  </si>
+  <si>
+    <t>http://3.65.165.176:8081/Xe/</t>
+  </si>
+  <si>
+    <t>List of Evn</t>
+  </si>
+  <si>
+    <t>http://3.127.88.99:8087/Xe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +148,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -219,6 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -559,17 +590,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="74.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
@@ -589,13 +620,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>8</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -606,16 +637,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G2" s="9"/>
     </row>
@@ -627,16 +658,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3" s="9"/>
     </row>
@@ -648,16 +679,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="9"/>
     </row>
@@ -669,16 +700,16 @@
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="9"/>
     </row>
@@ -690,16 +721,16 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" s="9"/>
     </row>
@@ -711,23 +742,84 @@
         <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="9"/>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="9"/>
+      <c r="D9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -755,24 +847,24 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -786,16 +878,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -803,25 +896,41 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
+        <v>30</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{9B3128C1-BCE3-49D2-907E-7EE4AE0BC3F1}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{33435D92-FE08-4660-BF0C-30206E9D9FEF}"/>
+    <hyperlink ref="F3" r:id="rId3" xr:uid="{3E37945D-04D2-44B3-AC69-A81F18884CAE}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{02B4360E-EB60-425E-B01F-116A39CB7DAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
First push after Admin Panel, Scheme Setup and Member Onborading for single member is done
</commit_message>
<xml_diff>
--- a/UFT Framework/Controller.xlsx
+++ b/UFT Framework/Controller.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EA1F12-4ECB-4BA9-AE94-4A9E57867D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F47CBE8-A1CE-4A60-B9BD-010C34946E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27120" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
   <si>
     <t>Browser</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Reporting Mode</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>Abhijit.Das@test.com</t>
   </si>
   <si>
@@ -100,9 +97,6 @@
     <t>07_Scheme_Setup_CreateNewScheme_Approve_Clone_Switch</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -116,6 +110,18 @@
   </si>
   <si>
     <t>http://3.127.88.99:8087/Xe</t>
+  </si>
+  <si>
+    <t>http://3.127.88.99:8081/Xe</t>
+  </si>
+  <si>
+    <t>Scheme_setup_configs_practice</t>
+  </si>
+  <si>
+    <t>Claim_And_Pesioners_Configurations</t>
+  </si>
+  <si>
+    <t>Warning</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -250,6 +256,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -590,11 +599,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +629,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>8</v>
@@ -637,16 +646,14 @@
         <v>7</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E2" s="9"/>
       <c r="F2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" s="9"/>
     </row>
@@ -658,16 +665,14 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E3" s="9"/>
       <c r="F3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" s="9"/>
     </row>
@@ -679,16 +684,14 @@
         <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E4" s="9"/>
       <c r="F4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="9"/>
     </row>
@@ -700,16 +703,14 @@
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E5" s="9"/>
       <c r="F5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" s="9"/>
     </row>
@@ -721,16 +722,14 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E6" s="9"/>
       <c r="F6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="9"/>
     </row>
@@ -742,16 +741,14 @@
         <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E7" s="9"/>
       <c r="F7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7" s="9"/>
     </row>
@@ -763,14 +760,14 @@
         <v>7</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8" s="9"/>
     </row>
@@ -782,16 +779,14 @@
         <v>7</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>11</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="9"/>
     </row>
@@ -803,18 +798,55 @@
         <v>7</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="9"/>
+      <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -850,21 +882,21 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -878,10 +910,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,41 +928,47 @@
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F3" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F4" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{9B3128C1-BCE3-49D2-907E-7EE4AE0BC3F1}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{33435D92-FE08-4660-BF0C-30206E9D9FEF}"/>
-    <hyperlink ref="F3" r:id="rId3" xr:uid="{3E37945D-04D2-44B3-AC69-A81F18884CAE}"/>
-    <hyperlink ref="F4" r:id="rId4" xr:uid="{02B4360E-EB60-425E-B01F-116A39CB7DAF}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{33435D92-FE08-4660-BF0C-30206E9D9FEF}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{3E37945D-04D2-44B3-AC69-A81F18884CAE}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{02B4360E-EB60-425E-B01F-116A39CB7DAF}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{2A1F9886-DE5B-49FE-87DB-9EEBA4F3A515}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{4515C7F5-C6C9-4D64-B358-6BAE7FA41D68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commits up to contributions
</commit_message>
<xml_diff>
--- a/UFT Framework/Controller.xlsx
+++ b/UFT Framework/Controller.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F47CBE8-A1CE-4A60-B9BD-010C34946E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{46189996-8B52-48BD-AC39-022701E12B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2700" yWindow="2700" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="1" r:id="rId1"/>
     <sheet name="Config" sheetId="2" r:id="rId2"/>
     <sheet name="Environment" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Controller!$A$1:$I$27</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="61">
   <si>
     <t>Browser</t>
   </si>
@@ -97,38 +101,116 @@
     <t>07_Scheme_Setup_CreateNewScheme_Approve_Clone_Switch</t>
   </si>
   <si>
+    <t>AppURL</t>
+  </si>
+  <si>
+    <t>http://3.65.165.176:8081/Xe/</t>
+  </si>
+  <si>
+    <t>List of Evn</t>
+  </si>
+  <si>
+    <t>http://3.127.88.99:8087/Xe</t>
+  </si>
+  <si>
+    <t>http://3.127.88.99:8081/Xe</t>
+  </si>
+  <si>
+    <t>Claim_And_Pesioners_Configurations</t>
+  </si>
+  <si>
+    <t>MemberAddSingleDistrict</t>
+  </si>
+  <si>
+    <t>Update_Member_Details_Add_Notes</t>
+  </si>
+  <si>
+    <t>Configure_Contribution_Rates</t>
+  </si>
+  <si>
+    <t>Contribution_Add_Single_Contribution</t>
+  </si>
+  <si>
+    <t>Contribution_Show_Batch_Details</t>
+  </si>
+  <si>
+    <t>ImportMemberEndorseMemberUpdates</t>
+  </si>
+  <si>
+    <t>Member_Configurations_Setup</t>
+  </si>
+  <si>
+    <t>Contribution_And_Balances_Configurations</t>
+  </si>
+  <si>
+    <t>New_Single_Member_And_Approve</t>
+  </si>
+  <si>
+    <t>MemberDocumentsChecklist</t>
+  </si>
+  <si>
+    <t>AddPaypoints_And_Paypoint_Branches</t>
+  </si>
+  <si>
+    <t>Add_Single_And_Batch_Traditional_Authority</t>
+  </si>
+  <si>
+    <t>Add_Beneficiaries_Batch</t>
+  </si>
+  <si>
+    <t>Contributions_Batch_Upload</t>
+  </si>
+  <si>
+    <t>Configs_Tie_Contribution_To_Receipts</t>
+  </si>
+  <si>
+    <t>MemberOnboarding</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>Contribution_Billing</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Issue is fixed - issue with locator</t>
+  </si>
+  <si>
+    <t>Script in progress</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>AppURL</t>
-  </si>
-  <si>
-    <t>http://3.65.165.176:8081/Xe/</t>
-  </si>
-  <si>
-    <t>List of Evn</t>
-  </si>
-  <si>
-    <t>http://3.127.88.99:8087/Xe</t>
-  </si>
-  <si>
-    <t>http://3.127.88.99:8081/Xe</t>
-  </si>
-  <si>
-    <t>Scheme_setup_configs_practice</t>
-  </si>
-  <si>
-    <t>Claim_And_Pesioners_Configurations</t>
-  </si>
-  <si>
-    <t>Warning</t>
+    <t>Data issue : there is no Aduit for delete operation</t>
+  </si>
+  <si>
+    <t>Currency type Euro not exist in the drop down changed the currency type to US DOLLAR</t>
+  </si>
+  <si>
+    <t>Issue with "turnOffLocationBreakdown" method - I think it's added by John, commented the method for now</t>
+  </si>
+  <si>
+    <t>Some of the objct not found in object repo - John can debug futher</t>
+  </si>
+  <si>
+    <t>Getting error as Obj elmSponsorCheckBox not found - John can debug further</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +247,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,6 +271,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -232,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -257,7 +376,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -599,23 +740,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="78.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -638,7 +779,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -649,15 +790,17 @@
         <v>22</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="F2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="9"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -668,15 +811,17 @@
         <v>17</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="F3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -687,15 +832,19 @@
         <v>18</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="F4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -706,15 +855,17 @@
         <v>19</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="F5" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -725,15 +876,17 @@
         <v>20</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="F6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -744,15 +897,19 @@
         <v>21</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="F7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -763,15 +920,17 @@
         <v>25</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="9"/>
+        <v>54</v>
+      </c>
+      <c r="E8" s="18"/>
       <c r="F8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -782,71 +941,400 @@
         <v>23</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="F9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="9"/>
+        <v>6</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="F10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="9"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D18" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="7"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>23</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="9"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>24</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="9"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>25</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="9"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
         <v>26</v>
       </c>
-      <c r="E11" s="9"/>
-      <c r="F11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="B26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>27</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -863,15 +1351,15 @@
       <selection activeCell="C4" sqref="A4:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -885,7 +1373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -916,48 +1404,48 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F4" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" s="5" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F5" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -971,4 +1459,63 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772B1656-754C-4953-AE58-866F94EEAD0A}">
+  <dimension ref="A2:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="7">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>28</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>